<commit_message>
quick 2 sample t test of emerita samples
</commit_message>
<xml_diff>
--- a/data/Diet_emerita_population_data_raw.xlsx
+++ b/data/Diet_emerita_population_data_raw.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crab Lab\Box\Crab Lab Group Folder\Seasonal and Diet Field Data\Data entered\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\Box\Crab Lab Group Folder\Seasonal and Diet Field Data\Data entered\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8071B34-5923-4A6A-A00D-301FADE810BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-110" yWindow="11890" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="1" r:id="rId1"/>
     <sheet name="Biomass" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Population!$A$1:$U$940</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Population!$A$1:$U$1094</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6547" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6635" uniqueCount="94">
   <si>
     <t>Site</t>
   </si>
@@ -323,7 +324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -640,13 +641,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1094"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1036" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="J901" sqref="J901"/>
+      <selection pane="bottomLeft" activeCell="I1044" sqref="I1044"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6484,6 +6485,9 @@
       <c r="M124">
         <v>2</v>
       </c>
+      <c r="N124" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O124">
         <f t="shared" si="4"/>
         <v>356.50623885918003</v>
@@ -6529,6 +6533,9 @@
       <c r="M125">
         <v>1</v>
       </c>
+      <c r="N125" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O125">
         <f t="shared" si="4"/>
         <v>178.25311942959001</v>
@@ -6574,6 +6581,9 @@
       <c r="M126">
         <v>1</v>
       </c>
+      <c r="N126" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O126">
         <f t="shared" si="4"/>
         <v>178.25311942959001</v>
@@ -6655,6 +6665,9 @@
       <c r="M128">
         <v>2</v>
       </c>
+      <c r="N128" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O128">
         <f t="shared" si="4"/>
         <v>356.50623885918003</v>
@@ -6694,6 +6707,9 @@
       <c r="M129">
         <v>1</v>
       </c>
+      <c r="N129" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O129">
         <f t="shared" si="4"/>
         <v>178.25311942959001</v>
@@ -7530,6 +7546,9 @@
       <c r="M147">
         <v>6</v>
       </c>
+      <c r="N147" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O147">
         <f t="shared" si="7"/>
         <v>534.75935828877004</v>
@@ -7572,6 +7591,9 @@
       <c r="M148">
         <v>2</v>
       </c>
+      <c r="N148" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O148">
         <f t="shared" si="7"/>
         <v>178.25311942959001</v>
@@ -7611,6 +7633,9 @@
       <c r="M149">
         <v>2</v>
       </c>
+      <c r="N149" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O149">
         <f t="shared" si="7"/>
         <v>178.25311942959001</v>
@@ -7650,6 +7675,9 @@
       <c r="M150">
         <v>1</v>
       </c>
+      <c r="N150" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O150">
         <f t="shared" si="7"/>
         <v>89.126559714795007</v>
@@ -8682,6 +8710,9 @@
       <c r="M172">
         <v>3</v>
       </c>
+      <c r="N172" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O172">
         <f t="shared" si="7"/>
         <v>267.37967914438502</v>
@@ -8721,6 +8752,9 @@
       <c r="M173">
         <v>1</v>
       </c>
+      <c r="N173" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O173">
         <f t="shared" si="7"/>
         <v>89.126559714795007</v>
@@ -9654,6 +9688,9 @@
       <c r="M193">
         <v>2</v>
       </c>
+      <c r="N193" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O193">
         <f t="shared" si="7"/>
         <v>356.50623885918003</v>
@@ -9693,6 +9730,9 @@
       <c r="M194">
         <v>5</v>
       </c>
+      <c r="N194" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O194">
         <f t="shared" si="7"/>
         <v>891.26559714795007</v>
@@ -9732,6 +9772,9 @@
       <c r="M195">
         <v>1</v>
       </c>
+      <c r="N195" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O195">
         <f t="shared" ref="O195:O258" si="10">M195*(H195/0.007854)</f>
         <v>178.25311942959001</v>
@@ -10424,6 +10467,9 @@
       <c r="M210">
         <v>2</v>
       </c>
+      <c r="N210" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O210">
         <f t="shared" si="10"/>
         <v>331.04150751209579</v>
@@ -10463,6 +10509,9 @@
       <c r="M211">
         <v>4</v>
       </c>
+      <c r="N211" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O211">
         <f t="shared" si="10"/>
         <v>662.08301502419158</v>
@@ -10502,6 +10551,9 @@
       <c r="M212">
         <v>1</v>
       </c>
+      <c r="N212" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O212">
         <f t="shared" si="10"/>
         <v>165.5207537560479</v>
@@ -11632,6 +11684,9 @@
       <c r="M236">
         <v>2</v>
       </c>
+      <c r="N236" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O236">
         <f t="shared" si="10"/>
         <v>152.78838808250572</v>
@@ -11671,6 +11726,9 @@
       <c r="M237">
         <v>3</v>
       </c>
+      <c r="N237" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O237">
         <f t="shared" si="10"/>
         <v>229.18258212375858</v>
@@ -11710,6 +11768,9 @@
       <c r="M238">
         <v>7</v>
       </c>
+      <c r="N238" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O238">
         <f t="shared" si="10"/>
         <v>534.75935828877004</v>
@@ -11749,6 +11810,9 @@
       <c r="M239">
         <v>1</v>
       </c>
+      <c r="N239" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O239">
         <f t="shared" si="10"/>
         <v>76.39419404125286</v>
@@ -12729,6 +12793,9 @@
       <c r="M260">
         <v>3</v>
       </c>
+      <c r="N260" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O260">
         <f t="shared" si="14"/>
         <v>229.18258212375858</v>
@@ -12768,6 +12835,9 @@
       <c r="M261">
         <v>3</v>
       </c>
+      <c r="N261" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O261">
         <f t="shared" si="14"/>
         <v>229.18258212375858</v>
@@ -14174,6 +14244,9 @@
       <c r="M291">
         <v>3</v>
       </c>
+      <c r="N291" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O291">
         <f t="shared" si="14"/>
         <v>229.18258212375858</v>
@@ -14213,6 +14286,9 @@
       <c r="M292">
         <v>7</v>
       </c>
+      <c r="N292" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O292">
         <f t="shared" si="14"/>
         <v>534.75935828877004</v>
@@ -14252,6 +14328,9 @@
       <c r="M293">
         <v>1</v>
       </c>
+      <c r="N293" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O293">
         <f t="shared" si="14"/>
         <v>76.39419404125286</v>
@@ -15048,6 +15127,9 @@
       <c r="M310">
         <v>1</v>
       </c>
+      <c r="N310" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O310">
         <f t="shared" si="14"/>
         <v>76.39419404125286</v>
@@ -15087,6 +15169,9 @@
       <c r="M311">
         <v>1</v>
       </c>
+      <c r="N311" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O311">
         <f t="shared" si="14"/>
         <v>76.39419404125286</v>
@@ -16398,6 +16483,9 @@
       <c r="M339">
         <v>3</v>
       </c>
+      <c r="N339" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O339">
         <f t="shared" si="18"/>
         <v>229.18258212375858</v>
@@ -16437,6 +16525,9 @@
       <c r="M340">
         <v>5</v>
       </c>
+      <c r="N340" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O340">
         <f t="shared" si="18"/>
         <v>381.97097020626427</v>
@@ -17460,6 +17551,9 @@
       <c r="M362">
         <v>8</v>
       </c>
+      <c r="N362" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O362">
         <f t="shared" si="18"/>
         <v>407.43570155334862</v>
@@ -17499,6 +17593,9 @@
       <c r="M363">
         <v>1</v>
       </c>
+      <c r="N363" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O363">
         <f t="shared" si="18"/>
         <v>50.929462694168578</v>
@@ -17538,6 +17635,9 @@
       <c r="M364">
         <v>3</v>
       </c>
+      <c r="N364" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O364">
         <f t="shared" si="18"/>
         <v>152.78838808250572</v>
@@ -17577,6 +17677,9 @@
       <c r="M365">
         <v>1</v>
       </c>
+      <c r="N365" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O365">
         <f t="shared" si="18"/>
         <v>50.929462694168578</v>
@@ -18655,6 +18758,9 @@
       <c r="M388">
         <v>3</v>
       </c>
+      <c r="N388" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O388">
         <f t="shared" si="21"/>
         <v>152.78838808250572</v>
@@ -18742,6 +18848,9 @@
       <c r="M390">
         <v>1</v>
       </c>
+      <c r="N390" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O390">
         <f t="shared" si="21"/>
         <v>50.929462694168578</v>
@@ -18781,6 +18890,9 @@
       <c r="M391">
         <v>1</v>
       </c>
+      <c r="N391" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O391">
         <f t="shared" si="21"/>
         <v>50.929462694168578</v>
@@ -18820,6 +18932,9 @@
       <c r="M392">
         <v>1</v>
       </c>
+      <c r="N392" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O392">
         <f t="shared" si="21"/>
         <v>50.929462694168578</v>
@@ -19898,6 +20013,9 @@
       <c r="M415">
         <v>7</v>
       </c>
+      <c r="N415" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O415">
         <f t="shared" si="21"/>
         <v>356.50623885918003</v>
@@ -21073,6 +21191,9 @@
       <c r="M440">
         <v>8</v>
       </c>
+      <c r="N440" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O440">
         <f t="shared" si="21"/>
         <v>407.43570155334862</v>
@@ -21166,6 +21287,9 @@
       <c r="M442">
         <v>1</v>
       </c>
+      <c r="N442" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O442">
         <f t="shared" si="21"/>
         <v>50.929462694168578</v>
@@ -21301,6 +21425,9 @@
       <c r="M445">
         <v>1</v>
       </c>
+      <c r="N445" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O445">
         <f t="shared" si="21"/>
         <v>50.929462694168578</v>
@@ -22419,6 +22546,9 @@
       <c r="M469">
         <v>7</v>
       </c>
+      <c r="N469" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O469">
         <f t="shared" si="25"/>
         <v>356.50623885918003</v>
@@ -23343,6 +23473,9 @@
       <c r="M489">
         <v>1</v>
       </c>
+      <c r="N489" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O489">
         <f t="shared" si="25"/>
         <v>63.661828367710719</v>
@@ -24317,6 +24450,9 @@
       <c r="M510">
         <v>2</v>
       </c>
+      <c r="N510" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O510">
         <f t="shared" si="25"/>
         <v>127.32365673542144</v>
@@ -25254,6 +25390,9 @@
       <c r="M530">
         <v>2</v>
       </c>
+      <c r="N530" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O530">
         <f t="shared" si="29"/>
         <v>127.32365673542144</v>
@@ -26427,6 +26566,9 @@
       <c r="M555">
         <v>1</v>
       </c>
+      <c r="N555" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O555">
         <f t="shared" si="29"/>
         <v>63.661828367710719</v>
@@ -27358,6 +27500,9 @@
       <c r="M575">
         <v>1</v>
       </c>
+      <c r="N575" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="O575">
         <f t="shared" si="29"/>
         <v>63.661828367710719</v>
@@ -28574,7 +28719,7 @@
         <v>0</v>
       </c>
       <c r="N604" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="O604">
         <f t="shared" si="32"/>
@@ -29586,6 +29731,9 @@
       <c r="M629">
         <v>13</v>
       </c>
+      <c r="N629" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="630" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
@@ -30496,6 +30644,9 @@
       <c r="M652">
         <v>3</v>
       </c>
+      <c r="N652" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="653" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
@@ -31287,6 +31438,9 @@
       <c r="M672">
         <v>1</v>
       </c>
+      <c r="N672" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="673" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
@@ -32324,6 +32478,9 @@
       <c r="M698">
         <v>3</v>
       </c>
+      <c r="N698" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="699" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
@@ -32356,6 +32513,9 @@
       <c r="M699">
         <v>1</v>
       </c>
+      <c r="N699" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P699">
         <v>0.43769999999999998</v>
       </c>
@@ -33438,6 +33598,9 @@
       <c r="M726">
         <v>1</v>
       </c>
+      <c r="N726" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="727" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
@@ -34556,6 +34719,9 @@
       <c r="M754">
         <v>14</v>
       </c>
+      <c r="N754" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="755" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
@@ -34588,6 +34754,9 @@
       <c r="M755">
         <v>1</v>
       </c>
+      <c r="N755" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P755">
         <v>6.8099999999999994E-2</v>
       </c>
@@ -34623,6 +34792,9 @@
       <c r="M756">
         <v>3</v>
       </c>
+      <c r="N756" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P756">
         <v>1.4961</v>
       </c>
@@ -35834,6 +36006,9 @@
       <c r="M786">
         <v>0</v>
       </c>
+      <c r="N786" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="787" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
@@ -36919,6 +37094,9 @@
       <c r="M813">
         <v>7</v>
       </c>
+      <c r="N813" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="814" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
@@ -36951,6 +37129,9 @@
       <c r="M814">
         <v>2</v>
       </c>
+      <c r="N814" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P814">
         <v>0.1991</v>
       </c>
@@ -38588,6 +38769,9 @@
       <c r="M856">
         <v>2</v>
       </c>
+      <c r="N856" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="857" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
@@ -38620,6 +38804,9 @@
       <c r="M857">
         <v>1</v>
       </c>
+      <c r="N857" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="858" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
@@ -38655,6 +38842,9 @@
       <c r="M858">
         <v>1</v>
       </c>
+      <c r="N858" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P858">
         <v>0.15229999999999999</v>
       </c>
@@ -38690,6 +38880,9 @@
       <c r="M859">
         <v>1</v>
       </c>
+      <c r="N859" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P859">
         <v>0.159</v>
       </c>
@@ -38725,6 +38918,9 @@
       <c r="M860">
         <v>2</v>
       </c>
+      <c r="N860" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P860">
         <v>4.9599999999999998E-2</v>
       </c>
@@ -39620,9 +39816,8 @@
       <c r="M883">
         <v>1</v>
       </c>
-      <c r="N883" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
+      <c r="N883" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="P883">
         <v>0.49320000000000003</v>
@@ -39659,9 +39854,8 @@
       <c r="M884">
         <v>2</v>
       </c>
-      <c r="N884" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
+      <c r="N884" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="P884">
         <v>8.6800000000000002E-2</v>
@@ -39698,9 +39892,8 @@
       <c r="M885">
         <v>2</v>
       </c>
-      <c r="N885" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
+      <c r="N885" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="P885">
         <v>4.4499999999999998E-2</v>
@@ -40325,9 +40518,8 @@
       <c r="M901">
         <v>2</v>
       </c>
-      <c r="N901" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
+      <c r="N901" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="902" spans="1:14" x14ac:dyDescent="0.25">
@@ -40403,9 +40595,8 @@
       <c r="M903">
         <v>2</v>
       </c>
-      <c r="N903" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
+      <c r="N903" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="904" spans="1:14" x14ac:dyDescent="0.25">
@@ -44789,6 +44980,9 @@
       <c r="M1015">
         <v>1</v>
       </c>
+      <c r="N1015" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1016" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
@@ -45207,6 +45401,9 @@
       <c r="M1026">
         <v>1</v>
       </c>
+      <c r="N1026" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1027" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
@@ -45239,6 +45436,9 @@
       <c r="M1027">
         <v>1</v>
       </c>
+      <c r="N1027" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1028" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
@@ -45496,6 +45696,9 @@
       <c r="M1034">
         <v>2</v>
       </c>
+      <c r="N1034" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1035" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
@@ -45569,6 +45772,9 @@
       <c r="M1036">
         <v>1</v>
       </c>
+      <c r="N1036" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1037" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
@@ -47106,6 +47312,9 @@
       <c r="M1077">
         <v>3</v>
       </c>
+      <c r="N1077" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1078" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1078" t="s">
@@ -47211,6 +47420,9 @@
       <c r="M1080">
         <v>2</v>
       </c>
+      <c r="N1080" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1081" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1081" t="s">
@@ -47243,6 +47455,9 @@
       <c r="M1081">
         <v>1</v>
       </c>
+      <c r="N1081" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1082" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1082" t="s">
@@ -47275,6 +47490,9 @@
       <c r="M1082">
         <v>1</v>
       </c>
+      <c r="N1082" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1083" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1083" t="s">
@@ -47307,6 +47525,9 @@
       <c r="M1083">
         <v>0</v>
       </c>
+      <c r="N1083" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="1084" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1084" t="s">
@@ -47339,6 +47560,9 @@
       <c r="M1084">
         <v>4</v>
       </c>
+      <c r="N1084" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1084" s="2"/>
     </row>
     <row r="1085" spans="1:16" x14ac:dyDescent="0.25">
@@ -47372,6 +47596,9 @@
       <c r="M1085">
         <v>1</v>
       </c>
+      <c r="N1085" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1085" s="2"/>
     </row>
     <row r="1086" spans="1:16" x14ac:dyDescent="0.25">
@@ -47405,6 +47632,9 @@
       <c r="M1086">
         <v>1</v>
       </c>
+      <c r="N1086" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1086" s="2"/>
     </row>
     <row r="1087" spans="1:16" x14ac:dyDescent="0.25">
@@ -47438,6 +47668,9 @@
       <c r="M1087">
         <v>1</v>
       </c>
+      <c r="N1087" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1087" s="2"/>
     </row>
     <row r="1088" spans="1:16" x14ac:dyDescent="0.25">
@@ -47549,6 +47782,9 @@
       <c r="M1090">
         <v>2</v>
       </c>
+      <c r="N1090" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1090" s="2"/>
     </row>
     <row r="1091" spans="1:16" x14ac:dyDescent="0.25">
@@ -47582,6 +47818,9 @@
       <c r="M1091">
         <v>1</v>
       </c>
+      <c r="N1091" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1091" s="2"/>
     </row>
     <row r="1092" spans="1:16" x14ac:dyDescent="0.25">
@@ -47615,7 +47854,7 @@
       <c r="M1092">
         <v>1</v>
       </c>
-      <c r="N1092">
+      <c r="N1092" s="3">
         <v>6.18</v>
       </c>
       <c r="P1092" s="2"/>
@@ -47651,7 +47890,9 @@
       <c r="M1093">
         <v>0</v>
       </c>
-      <c r="N1093"/>
+      <c r="N1093" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1093" s="2"/>
     </row>
     <row r="1094" spans="1:16" x14ac:dyDescent="0.25">
@@ -47685,10 +47926,13 @@
       <c r="M1094">
         <v>1</v>
       </c>
+      <c r="N1094" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P1094" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:U575">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U575">
     <sortCondition ref="A2:A575"/>
     <sortCondition ref="D2:D575"/>
     <sortCondition ref="C2:C575"/>
@@ -47703,7 +47947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R127"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>